<commit_message>
fixed not in garwood chunk and added woody species bci list (work in progress,  need to check woody synonyms)
</commit_message>
<xml_diff>
--- a/splists_out/zotz_species_not_in_garwood.xlsx
+++ b/splists_out/zotz_species_not_in_garwood.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,11 +378,6 @@
           <t>Sp (Croat 1978)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>is_garwood_synonym</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -405,9 +400,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -430,9 +422,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -455,9 +444,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -480,9 +466,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -505,9 +488,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -530,9 +510,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -555,9 +532,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -580,9 +554,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -605,9 +576,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -630,9 +598,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -655,9 +620,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -680,9 +642,6 @@
           <t>**</t>
         </is>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -704,9 +663,6 @@
         <is>
           <t>**</t>
         </is>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>